<commit_message>
resolved tab 16 report bugs
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_16_rpt_P_QuarterlyReview.xlsx
+++ b/backend/reports/xlsx/Tab_16_rpt_P_QuarterlyReview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD2C74A7-2BC1-924F-97FB-7EF386FC0FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF0A9F0-AFE2-EC48-9FC0-200615B8B831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,40 +36,173 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
-  <si>
-    <t>{#date=d.date}</t>
-  </si>
-  <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>{#fy=d.fiscal_year}</t>
-  </si>
-  <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+  <si>
+    <t>Project Information:</t>
+  </si>
+  <si>
+    <t>Budget Forecasting Information:</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Deliverables Name</t>
+  </si>
+  <si>
+    <t>Detail Amount</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Resp</t>
+  </si>
+  <si>
+    <t>Service Line</t>
+  </si>
+  <si>
+    <t>STOB</t>
+  </si>
+  <si>
+    <t>Financial Contact</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i+1]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Totals: </t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].detail_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].q1_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].q2_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].q3_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].q4_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i+1]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Manager: </t>
+  </si>
+  <si>
+    <t>{d.project.project_manager}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Name: </t>
+  </si>
+  <si>
+    <t>{d.project.project_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End Date: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project #: </t>
+  </si>
+  <si>
+    <t>{d.project.project_number}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Date: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As of {d.report_date}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year: </t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].fiscal_year}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Resource Type</t>
+  </si>
+  <si>
+    <t>Recovery Area</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].deliverable_name}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].id}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].detail_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].q1_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].q2_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].q3_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].q4_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].resource_type}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].responsibility}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].service_line}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].stob}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].expense_authority_name}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].porfolio_abbrev}</t>
+  </si>
+  <si>
+    <t>Fiscal Year Totals:</t>
+  </si>
+  <si>
+    <t>{d.project.planned_start_date:formatD(DD-MMM-YY)}</t>
+  </si>
+  <si>
+    <t>{d.project.planned_end_date:formatD(DD-MMM-YY)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Project Billing Quarterly Review Report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,31 +215,83 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF232731"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF232731"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF7E7E7E"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF404040"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF404040"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +306,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFD0D3DD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1F1F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -135,65 +332,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="0"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
+      <top style="thin">
+        <color theme="0"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
       </bottom>
       <diagonal/>
     </border>
@@ -201,49 +365,114 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,15 +502,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>107110</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>61205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:colOff>951057</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>282525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -310,8 +539,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2411054" cy="680356"/>
+          <a:off x="107110" y="61205"/>
+          <a:ext cx="2404670" cy="680356"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,9 +553,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +593,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -470,7 +699,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,7 +841,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,112 +852,360 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:XFD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="9" width="20.5" customWidth="1"/>
+    <col min="10" max="10" width="20.5" style="5" customWidth="1"/>
+    <col min="11" max="12" width="20.5" customWidth="1"/>
+    <col min="13" max="13" width="22.5" customWidth="1"/>
+    <col min="14" max="16383" width="20.5" hidden="1"/>
+    <col min="16384" max="16384" width="2.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="36" customHeight="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="36" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="28" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
+      <c r="I4" s="9"/>
+      <c r="J4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13" ht="34" customHeight="1">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+    </row>
+    <row r="6" spans="1:13" ht="28" customHeight="1">
+      <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" spans="1:13" ht="27" customHeight="1">
+      <c r="A7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+    </row>
+    <row r="8" spans="1:13" ht="39" customHeight="1">
+      <c r="A8" s="20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
+      <c r="B8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="F8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="34" customHeight="1">
+      <c r="A9" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="34" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+    </row>
+    <row r="11" spans="1:13" ht="66">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+    </row>
+    <row r="12" spans="1:13" ht="66">
+      <c r="A12" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+    </row>
+    <row r="13" spans="1:13" ht="21">
+      <c r="A13" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+    </row>
+    <row r="14" spans="1:13" hidden="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
resolved tab 16 report bugs (#730)
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_16_rpt_P_QuarterlyReview.xlsx
+++ b/backend/reports/xlsx/Tab_16_rpt_P_QuarterlyReview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aspiteri/Development/Github/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD2C74A7-2BC1-924F-97FB-7EF386FC0FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF0A9F0-AFE2-EC48-9FC0-200615B8B831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26660" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,40 +36,173 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>{#r=d.report[i]}</t>
-  </si>
-  <si>
-    <t>{#r1=d.report[i+1]}</t>
-  </si>
-  <si>
-    <t>{#t=d.report_totals[i]}</t>
-  </si>
-  <si>
-    <t>{#date=d.date}</t>
-  </si>
-  <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>{#fy=d.fiscal_year}</t>
-  </si>
-  <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
+  <si>
+    <t>Project Information:</t>
+  </si>
+  <si>
+    <t>Budget Forecasting Information:</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Deliverables Name</t>
+  </si>
+  <si>
+    <t>Detail Amount</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Resp</t>
+  </si>
+  <si>
+    <t>Service Line</t>
+  </si>
+  <si>
+    <t>STOB</t>
+  </si>
+  <si>
+    <t>Financial Contact</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i+1]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Client Totals: </t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].detail_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].q1_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].q2_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].q3_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].q4_client_total}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i+1]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Manager: </t>
+  </si>
+  <si>
+    <t>{d.project.project_manager}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Name: </t>
+  </si>
+  <si>
+    <t>{d.project.project_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End Date: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project #: </t>
+  </si>
+  <si>
+    <t>{d.project.project_number}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Date: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> As of {d.report_date}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiscal Year: </t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].fiscal_year}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Resource Type</t>
+  </si>
+  <si>
+    <t>Recovery Area</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].deliverable_name}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].id}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].detail_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].q1_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].q2_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].q3_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].q4_amount}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].resource_type}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].responsibility}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].service_line}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].stob}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].expense_authority_name}</t>
+  </si>
+  <si>
+    <t>{d.deliverables[i].details[i].porfolio_abbrev}</t>
+  </si>
+  <si>
+    <t>Fiscal Year Totals:</t>
+  </si>
+  <si>
+    <t>{d.project.planned_start_date:formatD(DD-MMM-YY)}</t>
+  </si>
+  <si>
+    <t>{d.project.planned_end_date:formatD(DD-MMM-YY)}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Project Billing Quarterly Review Report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="7">
+  <fonts count="15">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,31 +215,83 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF232731"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF232731"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF7E7E7E"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF404040"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF404040"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -121,12 +306,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor rgb="FFD0D3DD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1F1F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -135,65 +332,32 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="0"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="0"/>
       </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
+      <top style="thin">
+        <color theme="0"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
       </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFA5A5A5"/>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFA5A5A5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
       </bottom>
       <diagonal/>
     </border>
@@ -201,49 +365,114 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,15 +502,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>107110</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>61205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>680356</xdr:rowOff>
+      <xdr:colOff>951057</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>282525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -310,8 +539,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="2411054" cy="680356"/>
+          <a:off x="107110" y="61205"/>
+          <a:ext cx="2404670" cy="680356"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -324,9 +553,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +593,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -470,7 +699,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -612,7 +841,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -623,112 +852,360 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:XFD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I2" sqref="C2:I2"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="9" width="20.5" customWidth="1"/>
+    <col min="10" max="10" width="20.5" style="5" customWidth="1"/>
+    <col min="11" max="12" width="20.5" customWidth="1"/>
+    <col min="13" max="13" width="22.5" customWidth="1"/>
+    <col min="14" max="16383" width="20.5" hidden="1"/>
+    <col min="16384" max="16384" width="2.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="36" customHeight="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" s="2" customFormat="1" ht="36" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+    </row>
+    <row r="3" spans="1:13" s="2" customFormat="1" ht="28" customHeight="1">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="4" t="s">
+      <c r="I4" s="9"/>
+      <c r="J4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13" ht="34" customHeight="1">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+    </row>
+    <row r="6" spans="1:13" ht="28" customHeight="1">
+      <c r="A6" s="15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="4" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+    </row>
+    <row r="7" spans="1:13" ht="27" customHeight="1">
+      <c r="A7" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+    </row>
+    <row r="8" spans="1:13" ht="39" customHeight="1">
+      <c r="A8" s="20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="4" t="s">
+      <c r="B8" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="F8" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="34" customHeight="1">
+      <c r="A9" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="34" customHeight="1">
+      <c r="A10" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+    </row>
+    <row r="11" spans="1:13" ht="66">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+    </row>
+    <row r="12" spans="1:13" ht="66">
+      <c r="A12" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+    </row>
+    <row r="13" spans="1:13" ht="21">
+      <c r="A13" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+    </row>
+    <row r="14" spans="1:13" hidden="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A6:M6"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
DESCW-2397 fix financial contact name on report model & template
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_16_rpt_P_QuarterlyReview.xlsx
+++ b/backend/reports/xlsx/Tab_16_rpt_P_QuarterlyReview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BD051B2-59DC-F341-9DD9-F18975A3A568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2DA2B0-05E4-C048-95E5-A0AA5E85C2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="rpt_P_QuarterlyReview" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t>{$rdcd.id}</t>
   </si>
   <si>
-    <t>{$rdcd.expense_authority_name}</t>
-  </si>
-  <si>
     <t>{#rdcd1= d.report[i].details.clients[i].data[i+1]}</t>
   </si>
   <si>
@@ -243,6 +240,9 @@
   </si>
   <si>
     <t>{#rgt1 = d.report[i+1].details.totals}</t>
+  </si>
+  <si>
+    <t>{$rdcd.financial_contact_name}</t>
   </si>
 </sst>
 </file>
@@ -460,15 +460,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -482,12 +473,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -500,6 +485,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -883,8 +883,8 @@
   </sheetPr>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1"/>
@@ -900,9 +900,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="65" customHeight="1">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="16" t="s">
+      <c r="A1" s="23"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D1" s="10"/>
@@ -912,26 +912,26 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="28" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="4" t="s">
@@ -943,22 +943,22 @@
       <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="15" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="13" t="s">
+      <c r="J3" s="22"/>
+      <c r="K3" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
     </row>
     <row r="4" spans="1:13" ht="34" customHeight="1">
       <c r="A4" s="4" t="s">
@@ -983,9 +983,9 @@
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:13" s="17" customFormat="1" ht="34" customHeight="1">
-      <c r="A5" s="17" t="s">
-        <v>65</v>
+    <row r="5" spans="1:13" s="14" customFormat="1" ht="34" customHeight="1">
+      <c r="A5" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="39" customHeight="1">
@@ -1029,219 +1029,219 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="15" customFormat="1" ht="34" customHeight="1">
-      <c r="A7" s="15" t="s">
+    <row r="7" spans="1:13" s="12" customFormat="1" ht="34" customHeight="1">
+      <c r="A7" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="D7" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="E7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="G7" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="H7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="I7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="J7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="K7" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="L7" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="M7" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="12" customFormat="1" ht="34" customHeight="1">
+      <c r="A8" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="44">
+      <c r="A9" s="20"/>
+      <c r="B9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="1:13" s="12" customFormat="1" ht="34" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="44">
+      <c r="A11" s="16"/>
+      <c r="B11" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="1:13" s="14" customFormat="1" ht="34" customHeight="1">
+      <c r="A12" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="21">
+      <c r="A13" s="12"/>
+    </row>
+    <row r="14" spans="1:13" ht="21">
+      <c r="A14" s="12"/>
+    </row>
+    <row r="15" spans="1:13" ht="21">
+      <c r="A15" s="12"/>
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:13" ht="21">
+      <c r="A16" s="12"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="11"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="15" t="s">
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="15" customFormat="1" ht="34" customHeight="1">
-      <c r="A8" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="44">
-      <c r="A9" s="25"/>
-      <c r="B9" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-    </row>
-    <row r="10" spans="1:13" s="15" customFormat="1" ht="34" customHeight="1">
-      <c r="A10" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="44">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-    </row>
-    <row r="12" spans="1:13" s="17" customFormat="1" ht="34" customHeight="1">
-      <c r="A12" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="21">
-      <c r="A13" s="15"/>
-    </row>
-    <row r="14" spans="1:13" ht="21">
-      <c r="A14" s="15"/>
-    </row>
-    <row r="15" spans="1:13" ht="21">
-      <c r="A15" s="15"/>
-      <c r="F15" s="24"/>
-    </row>
-    <row r="16" spans="1:13" ht="21">
-      <c r="A16" s="15"/>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2">
-      <c r="B22" s="14"/>
-    </row>
-    <row r="23" spans="2:2">
-      <c r="B23" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" s="14" t="s">
+    <row r="27" spans="2:2">
+      <c r="B27" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="2:2">
-      <c r="B25" s="14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2">
-      <c r="B26" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2">
-      <c r="B27" s="14" t="s">
+    <row r="28" spans="2:2">
+      <c r="B28" s="11" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" s="14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="29" spans="2:2"/>
     <row r="30" spans="2:2">
-      <c r="B30" s="14" t="s">
-        <v>58</v>
+      <c r="B30" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:2">
-      <c r="B31" s="14" t="s">
-        <v>64</v>
+      <c r="B31" s="11" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="2:2">
-      <c r="B32" s="14"/>
+      <c r="B32" s="11"/>
     </row>
     <row r="33" spans="2:2">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
     <row r="35" spans="2:2" hidden="1">
-      <c r="B35" s="14"/>
+      <c r="B35" s="11"/>
     </row>
     <row r="37" spans="2:2" hidden="1">
-      <c r="B37" s="14"/>
+      <c r="B37" s="11"/>
     </row>
     <row r="38" spans="2:2" hidden="1">
-      <c r="B38" s="14"/>
+      <c r="B38" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>